<commit_message>
Fix Bug and add carosel admin panel
</commit_message>
<xml_diff>
--- a/CarVendor.Web/Content/Uploads/SIG_.xlsx
+++ b/CarVendor.Web/Content/Uploads/SIG_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="88">
   <si>
     <t>EngineCapacity</t>
   </si>
@@ -280,9 +280,6 @@
   </si>
   <si>
     <t>NULL</t>
-  </si>
-  <si>
-    <t>Mageeeed</t>
   </si>
   <si>
     <t>0</t>
@@ -607,7 +604,7 @@
   <dimension ref="A1:CH2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -877,7 +874,7 @@
     </row>
     <row r="2" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
@@ -895,7 +892,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H2" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
privacy policy and terms of service
</commit_message>
<xml_diff>
--- a/CarVendor.Web/Content/Uploads/SIG_.xlsx
+++ b/CarVendor.Web/Content/Uploads/SIG_.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CB8245-014A-4407-A68A-595DC5799F31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="89">
   <si>
     <t>EngineCapacity</t>
   </si>
@@ -283,12 +284,15 @@
   </si>
   <si>
     <t>0</t>
+  </si>
+  <si>
+    <t>ahmed ebrahem</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -600,7 +604,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CH2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -892,7 +896,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H2" s="1">
         <v>0</v>

</xml_diff>